<commit_message>
updates on the protocol scripts
</commit_message>
<xml_diff>
--- a/Data_processing/C_elegans/example_files/Snoek_2019_marker01.xlsx
+++ b/Data_processing/C_elegans/example_files/Snoek_2019_marker01.xlsx
@@ -297,10 +297,13 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="187" zoomScaleNormal="187" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.65"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>